<commit_message>
Cập nhật file Mo_ta_cong_viec.xlsx
</commit_message>
<xml_diff>
--- a/Mo_ta_cong_viec.xlsx
+++ b/Mo_ta_cong_viec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uhvtran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvnva\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51B85E00-F977-40EC-83CC-AF9708B23476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506EC763-F3D7-4CD3-B7D7-C547473E86BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10FA5675-7159-4755-B639-418A7E1D35AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>STT</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>gặp online</t>
+  </si>
+  <si>
+    <t>Tìm hiểu đề tài, công nghệ sử dụng, vẽ sơ đồ uscase tổng quát</t>
+  </si>
+  <si>
+    <t>mô tả usecase, làm sơ đồ erd</t>
   </si>
 </sst>
 </file>
@@ -194,13 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -208,8 +212,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,9 +231,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +271,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -374,7 +377,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,7 +530,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,60 +542,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="1"/>
@@ -601,13 +608,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="1"/>
@@ -616,13 +623,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="1"/>
@@ -631,13 +638,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1"/>
@@ -646,13 +653,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="1"/>
@@ -661,13 +668,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1"/>
@@ -676,13 +683,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="1"/>
@@ -691,13 +698,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="1"/>
@@ -706,13 +713,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="1"/>
@@ -721,13 +728,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="1"/>
@@ -736,13 +743,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="1"/>
@@ -751,13 +758,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1"/>
@@ -766,10 +773,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">

</xml_diff>